<commit_message>
Added subs for l.sb and l.sh
</commit_message>
<xml_diff>
--- a/res/insn_groups.xlsx
+++ b/res/insn_groups.xlsx
@@ -861,8 +861,8 @@
   </sheetPr>
   <dimension ref="A1:P110"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L38" activeCellId="0" sqref="L38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A57" activeCellId="0" sqref="A57:G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1963,61 +1963,61 @@
       <c r="G56" s="5"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="6" t="s">
+      <c r="A57" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B57" s="0" t="n">
+      <c r="B57" s="8" t="n">
         <v>55</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C57" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D57" s="6" t="s">
+      <c r="D57" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E57" s="6" t="s">
+      <c r="E57" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="F57" s="6"/>
-      <c r="G57" s="6"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="6" t="s">
+      <c r="A58" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B58" s="0" t="n">
+      <c r="B58" s="8" t="n">
         <v>56</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C58" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D58" s="6" t="s">
+      <c r="D58" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E58" s="6" t="s">
+      <c r="E58" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="F58" s="6"/>
-      <c r="G58" s="6"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B59" s="0" t="n">
+      <c r="B59" s="8" t="n">
         <v>57</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C59" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D59" s="6" t="s">
+      <c r="D59" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E59" s="6" t="s">
+      <c r="E59" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="F59" s="6"/>
-      <c r="G59" s="6"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
@@ -2066,94 +2066,94 @@
       </c>
     </row>
     <row r="62" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="7" t="s">
+      <c r="A62" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B62" s="7" t="n">
+      <c r="B62" s="2" t="n">
         <v>60</v>
       </c>
-      <c r="C62" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="D62" s="7" t="s">
+      <c r="C62" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E62" s="7" t="s">
+      <c r="E62" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F62" s="7" t="s">
+      <c r="F62" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G62" s="7" t="s">
+      <c r="G62" s="2" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="7" t="s">
+      <c r="A63" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B63" s="8" t="n">
+      <c r="B63" s="0" t="n">
         <v>61</v>
       </c>
-      <c r="C63" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="D63" s="7" t="s">
+      <c r="C63" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D63" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E63" s="7" t="s">
+      <c r="E63" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F63" s="7" t="s">
+      <c r="F63" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G63" s="7" t="s">
+      <c r="G63" s="2" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="7" t="s">
+      <c r="A64" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B64" s="8" t="n">
+      <c r="B64" s="0" t="n">
         <v>62</v>
       </c>
-      <c r="C64" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="D64" s="7" t="s">
+      <c r="C64" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D64" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E64" s="7" t="s">
+      <c r="E64" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F64" s="7" t="s">
+      <c r="F64" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G64" s="7" t="s">
+      <c r="G64" s="2" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="7" t="s">
+      <c r="A65" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B65" s="8" t="n">
+      <c r="B65" s="0" t="n">
         <v>63</v>
       </c>
-      <c r="C65" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="D65" s="7" t="s">
+      <c r="C65" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D65" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E65" s="7" t="s">
+      <c r="E65" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F65" s="7" t="s">
+      <c r="F65" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G65" s="7" t="s">
+      <c r="G65" s="2" t="s">
         <v>132</v>
       </c>
     </row>

</xml_diff>